<commit_message>
load renter data by column name instead of column number
</commit_message>
<xml_diff>
--- a/src/main/resources/Indexmieten_Übersicht.xlsx
+++ b/src/main/resources/Indexmieten_Übersicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\IdeaProjects\rent-index\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7A2A882-3100-4F31-B743-940018F62365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2CCDF7-E5DA-46AF-AAD8-E2015C852438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
     <t>Wfl.m2</t>
   </si>
   <si>
-    <t>Balk.</t>
-  </si>
-  <si>
     <t>Lage</t>
   </si>
   <si>
@@ -46,9 +43,6 @@
     <t>Zustand</t>
   </si>
   <si>
-    <t>Beheizg.</t>
-  </si>
-  <si>
     <t>Ausgesetzt</t>
   </si>
   <si>
@@ -182,6 +176,12 @@
   </si>
   <si>
     <t>Lambrecht</t>
+  </si>
+  <si>
+    <t>Balkon</t>
+  </si>
+  <si>
+    <t>Beheizung</t>
   </si>
 </sst>
 </file>
@@ -272,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -299,8 +299,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -606,7 +604,7 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -633,104 +631,104 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>52</v>
+      <c r="A2" t="s">
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="2">
         <v>44</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
       </c>
       <c r="K2">
         <v>2023</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M2">
         <v>720</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:N29" si="0">ROUND(M2/D2, 2)</f>
+        <f t="shared" ref="N2:N3" si="0">ROUND(M2/D2, 2)</f>
         <v>16.36</v>
       </c>
       <c r="O2">
@@ -738,33 +736,33 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
-        <v>46</v>
+      <c r="A3" t="s">
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2">
         <v>64</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K3">
         <v>2022</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M3">
         <v>945</v>
@@ -778,39 +776,39 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" s="5">
         <v>104</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K4">
         <v>2023</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M4">
         <v>1345</v>
@@ -824,36 +822,36 @@
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
-        <v>43</v>
+      <c r="A5" t="s">
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" s="5">
         <v>74</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K5">
         <v>2022</v>
       </c>
       <c r="L5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M5">
         <v>1122</v>
@@ -870,33 +868,33 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>50</v>
+      <c r="A6" t="s">
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" s="5">
         <v>34</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K6">
         <v>2023</v>
       </c>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M6">
         <v>544</v>
@@ -913,55 +911,43 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
       <c r="D7" s="2"/>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
-    </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A12" s="12"/>
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A13" s="12"/>
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A17" s="13"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
@@ -984,26 +970,20 @@
       <c r="W17" s="7"/>
       <c r="X17" s="7"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-    </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A20" s="12"/>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A21" s="12"/>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A22" s="13"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
@@ -1025,21 +1005,15 @@
       <c r="W22" s="7"/>
       <c r="X22" s="7"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
-    </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A25" s="12"/>
       <c r="D25" s="5"/>
       <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
     </row>

</xml_diff>